<commit_message>
Fix DNXL Export: Smart clear to preserve footer + STT starts from 1
</commit_message>
<xml_diff>
--- a/templates/Template_DNXL.xlsx
+++ b/templates/Template_DNXL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thành\Work\Antigravity\NCR_mobile_project\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thành\Work\Antigravity\NCR_mobile_project\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8E1061-EE95-4DDD-92CF-4583FB0E5CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916733BD-ADA4-4236-8FED-002826D856E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31695" yWindow="45" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29685" yWindow="-705" windowWidth="21600" windowHeight="16200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="old" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="73">
   <si>
     <t xml:space="preserve">                                CÔNG TY CỔ PHẦN BAO BÌ ĐẠI LỤC
                                 Continent Packaging Corporation</t>
@@ -330,9 +330,6 @@
   </si>
   <si>
     <t>{{ i.ten_loi }}</t>
-  </si>
-  <si>
-    <t>{{ tong_sl_dat }}</t>
   </si>
 </sst>
 </file>
@@ -677,9 +674,45 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -689,41 +722,44 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -748,45 +784,6 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1241,185 +1238,185 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="31" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
       <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31" t="s">
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
       <c r="J2" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31" t="s">
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
       <c r="J3" s="3">
         <v>43850</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="31" t="s">
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
       <c r="J4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
     </row>
     <row r="6" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
     </row>
     <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30" t="s">
+      <c r="B7" s="40"/>
+      <c r="C7" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30" t="s">
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
       <c r="J7" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30" t="s">
+      <c r="B8" s="40"/>
+      <c r="C8" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30" t="s">
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
     </row>
     <row r="9" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30" t="s">
+      <c r="B9" s="40"/>
+      <c r="C9" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30" t="s">
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
     </row>
     <row r="10" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="35" t="s">
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35" t="s">
+      <c r="H10" s="42"/>
+      <c r="I10" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="35" t="s">
+      <c r="J10" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="37"/>
+      <c r="K10" s="31"/>
     </row>
     <row r="11" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="41"/>
       <c r="C11" s="6" t="s">
         <v>21</v>
       </c>
@@ -1438,9 +1435,9 @@
       <c r="H11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="37"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="31"/>
     </row>
     <row r="12" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
@@ -1569,50 +1566,50 @@
       <c r="J21" s="12"/>
     </row>
     <row r="22" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="38"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
     </row>
     <row r="23" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
     </row>
     <row r="24" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="39" t="s">
+      <c r="B24" s="35"/>
+      <c r="C24" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39" t="s">
+      <c r="D24" s="33"/>
+      <c r="E24" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
@@ -1622,7 +1619,7 @@
       <c r="E25" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="42" t="s">
+      <c r="F25" s="36" t="s">
         <v>30</v>
       </c>
       <c r="G25" s="21" t="s">
@@ -1638,7 +1635,7 @@
       <c r="E26" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="43"/>
+      <c r="F26" s="37"/>
       <c r="G26" s="23" t="s">
         <v>33</v>
       </c>
@@ -1652,7 +1649,7 @@
       <c r="E27" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="44"/>
+      <c r="F27" s="38"/>
       <c r="G27" s="25" t="s">
         <v>35</v>
       </c>
@@ -1661,28 +1658,28 @@
       <c r="J27" s="25"/>
     </row>
     <row r="28" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="45"/>
-      <c r="B28" s="45"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="39"/>
     </row>
     <row r="29" spans="1:12" s="26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36" t="s">
+      <c r="B29" s="30"/>
+      <c r="C29" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36" t="s">
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36" t="s">
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="J29" s="36"/>
+      <c r="J29" s="30"/>
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1693,6 +1690,29 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="A1:F4"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="K10:K11"/>
     <mergeCell ref="A22:B22"/>
@@ -1707,29 +1727,6 @@
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="F29:H29"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="A1:F4"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:I7"/>
   </mergeCells>
   <pageMargins left="0.43" right="0.17" top="0.17" bottom="0.17" header="0.17" footer="0.17"/>
   <pageSetup scale="95" orientation="portrait" r:id="rId1"/>
@@ -1744,8 +1741,8 @@
   </sheetPr>
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1760,178 +1757,178 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="48" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="49"/>
-      <c r="I1" s="48" t="s">
+      <c r="H1" s="62"/>
+      <c r="I1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="50"/>
-      <c r="K1" s="49"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="62"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="48" t="s">
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="48">
+      <c r="H2" s="62"/>
+      <c r="I2" s="61">
         <v>3</v>
       </c>
-      <c r="J2" s="50"/>
-      <c r="K2" s="49"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="62"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="48" t="s">
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="49"/>
-      <c r="I3" s="51">
+      <c r="H3" s="62"/>
+      <c r="I3" s="64">
         <v>45637</v>
       </c>
-      <c r="J3" s="52"/>
-      <c r="K3" s="53"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="66"/>
     </row>
     <row r="4" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
     </row>
     <row r="5" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30" t="s">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
     </row>
     <row r="6" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="64" t="s">
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="H6" s="65"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="64" t="s">
+      <c r="H6" s="51"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="K6" s="66"/>
+      <c r="K6" s="52"/>
     </row>
     <row r="7" spans="1:12" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63" t="s">
+      <c r="B7" s="49"/>
+      <c r="C7" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63" t="s">
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="63"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
     </row>
     <row r="8" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30" t="s">
+      <c r="B8" s="40"/>
+      <c r="C8" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30" t="s">
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
     </row>
     <row r="9" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="56"/>
-      <c r="E9" s="55" t="s">
+      <c r="D9" s="55"/>
+      <c r="E9" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="56"/>
+      <c r="F9" s="55"/>
       <c r="G9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="57" t="s">
+      <c r="H9" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="37"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="31"/>
     </row>
     <row r="10" spans="1:12" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
       <c r="C10" s="6" t="s">
         <v>23</v>
       </c>
@@ -1959,7 +1956,7 @@
       <c r="K10" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="L10" s="37"/>
+      <c r="L10" s="31"/>
     </row>
     <row r="11" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
@@ -2128,75 +2125,73 @@
       <c r="K22" s="12"/>
     </row>
     <row r="23" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
     </row>
     <row r="24" spans="1:13" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="38"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
     </row>
     <row r="25" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="41"/>
-      <c r="C25" s="39" t="s">
+      <c r="B25" s="35"/>
+      <c r="C25" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="60" t="s">
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="I25" s="61"/>
-      <c r="J25" s="61"/>
-      <c r="K25" s="62"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="48"/>
     </row>
     <row r="26" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="45"/>
-      <c r="B26" s="45"/>
+      <c r="A26" s="39"/>
+      <c r="B26" s="39"/>
     </row>
     <row r="27" spans="1:13" s="26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36" t="s">
+      <c r="B27" s="30"/>
+      <c r="C27" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36" t="s">
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H27" s="36"/>
+      <c r="H27" s="30"/>
       <c r="J27" s="26" t="s">
         <v>52</v>
       </c>
@@ -2210,27 +2205,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:K5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:K23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:K24"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="H9:K9"/>
     <mergeCell ref="A1:F3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="G27:H27"/>
@@ -2247,6 +2221,27 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="G8:K8"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:K23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:K24"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:K5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="J6:K6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.59055118110236227" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.15748031496062992" footer="0.15748031496062992"/>

</xml_diff>